<commit_message>
Mail code added to the code
</commit_message>
<xml_diff>
--- a/tut06/output/2001CB02.xlsx
+++ b/tut06/output/2001CB02.xlsx
@@ -506,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -726,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -746,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -806,7 +806,7 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>